<commit_message>
Added a pivot table to the excel file - league summary by state
</commit_message>
<xml_diff>
--- a/Project 3 Prototype/major_teams_usa.xlsx
+++ b/Project 3 Prototype/major_teams_usa.xlsx
@@ -5,20 +5,24 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8af7e8536f9e44ec/Desktop/Project 3 Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8af7e8536f9e44ec/Desktop/Data Bootcamp/Project-3-Sports-Betting-Analysis/Project 3 Prototype/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{989FFF68-7F55-4867-B3DC-C13ED68D56D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03A8160E-B20A-4711-BC51-B64AC9696A26}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{989FFF68-7F55-4867-B3DC-C13ED68D56D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CBF29BD4-982E-49A0-B0CA-D83555E087A0}"/>
   <bookViews>
     <workbookView xWindow="43080" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FC46803A-E082-41A8-A115-835C1D64F664}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$143</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$E$143</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="3" r:id="rId3"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="376">
   <si>
     <t>Team</t>
   </si>
@@ -1155,6 +1159,18 @@
   </si>
   <si>
     <t>District of Columbia</t>
+  </si>
+  <si>
+    <t>Column Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Count of Team</t>
   </si>
 </sst>
 </file>
@@ -1190,8 +1206,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1209,8 +1230,1261 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Ludwika Lasota" refreshedDate="45155.866007407407" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="142" xr:uid="{0FD68F0D-4B45-49B5-B6C1-A25133D454F8}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:E143" sheet="Sheet1"/>
+  </cacheSource>
+  <cacheFields count="5">
+    <cacheField name="Team" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Venue" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="City" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="State/Province" numFmtId="0">
+      <sharedItems count="28">
+        <s v="Arizona"/>
+        <s v="California"/>
+        <s v="Colorado"/>
+        <s v="District of Columbia"/>
+        <s v="Florida"/>
+        <s v="Georgia"/>
+        <s v="Illinois"/>
+        <s v="Indiana"/>
+        <s v="Kansas"/>
+        <s v="Louisiana"/>
+        <s v="Maryland"/>
+        <s v="Massachusetts"/>
+        <s v="Michigan"/>
+        <s v="Minnesota"/>
+        <s v="Missouri"/>
+        <s v="Nevada"/>
+        <s v="New Jersey"/>
+        <s v="New York"/>
+        <s v="North Carolina"/>
+        <s v="Ohio"/>
+        <s v="Oklahoma"/>
+        <s v="Oregon"/>
+        <s v="Pennsylvania"/>
+        <s v="Tennessee"/>
+        <s v="Texas"/>
+        <s v="Utah"/>
+        <s v="Washington"/>
+        <s v="Wisconsin"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="League" numFmtId="0">
+      <sharedItems count="5">
+        <s v="MLB"/>
+        <s v="NBA"/>
+        <s v="NFL"/>
+        <s v="NHL"/>
+        <s v="MLS"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="142">
+  <r>
+    <s v="Arizona Diamondbacks"/>
+    <s v="Chase Field"/>
+    <s v="Phoenix"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Phoenix Suns"/>
+    <s v="Footprint Center"/>
+    <s v="Phoenix"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Arizona Cardinals"/>
+    <s v="State Farm Stadium"/>
+    <s v="Glendale"/>
+    <x v="0"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="Arizona Coyotes"/>
+    <s v="Mullett Arena"/>
+    <s v="Tempe"/>
+    <x v="0"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <s v="Anaheim Ducks"/>
+    <s v="Honda Center"/>
+    <s v="Anaheim"/>
+    <x v="1"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <s v="LA Galaxy"/>
+    <s v="Dignity Health Sports Park"/>
+    <s v="Carson"/>
+    <x v="1"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="Los Angeles FC"/>
+    <s v="Banc of California Stadium"/>
+    <s v="Los Angeles"/>
+    <x v="1"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="Los Angeles Kings"/>
+    <s v="Crypto.com Arena"/>
+    <s v="Los Angeles"/>
+    <x v="1"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <s v="San Diego Padres"/>
+    <s v="Petco Park"/>
+    <s v="San Diego"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="San Francisco 49ers"/>
+    <s v="Levi's Stadium"/>
+    <s v="Santa Clara"/>
+    <x v="1"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="San Jose Sharks"/>
+    <s v="SAP Center at San Jose"/>
+    <s v="San Jose"/>
+    <x v="1"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <s v="San Diego MLS team"/>
+    <s v="Snapdragon Stadium"/>
+    <s v="San Diego"/>
+    <x v="1"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="Los Angeles Chargers"/>
+    <s v="SoFi Stadium"/>
+    <s v="Inglewood"/>
+    <x v="1"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="Los Angeles Angels"/>
+    <s v="Angel Stadium"/>
+    <s v="Anaheim"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Los Angeles Dodgers"/>
+    <s v="Dodger Stadium"/>
+    <s v="Los Angeles"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Los Angeles Clippers"/>
+    <s v="Crypto.com Arena"/>
+    <s v="Los Angeles"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Los Angeles Rams"/>
+    <s v="SoFi Stadium"/>
+    <s v="Inglewood"/>
+    <x v="1"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="Los Angeles Lakers"/>
+    <s v="Crypto.com Arena"/>
+    <s v="Los Angeles"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="San Francisco Giants"/>
+    <s v="Oracle Park"/>
+    <s v="San Francisco"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Oakland Athletics"/>
+    <s v="Oakland Coliseum"/>
+    <s v="Oakland"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Golden State Warriors"/>
+    <s v="Chase Center"/>
+    <s v="San Francisco"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Sacramento Kings"/>
+    <s v="Golden 1 Center"/>
+    <s v="Sacramento"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="San Jose Earthquakes"/>
+    <s v="PayPal Park"/>
+    <s v="San Jose"/>
+    <x v="1"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="Colorado Rapids"/>
+    <s v="Dick's Sporting Goods Park"/>
+    <s v="Commerce City"/>
+    <x v="2"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="Colorado Rockies"/>
+    <s v="Coors Field"/>
+    <s v="Denver"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Denver Broncos"/>
+    <s v="Empower Field at Mile High"/>
+    <s v="Denver"/>
+    <x v="2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="Denver Nuggets"/>
+    <s v="Ball Arena"/>
+    <s v="Denver"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Colorado Avalanche"/>
+    <s v="Ball Arena"/>
+    <s v="Denver"/>
+    <x v="2"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <s v="D.C. United"/>
+    <s v="Audi Field"/>
+    <s v="Washington"/>
+    <x v="3"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="Washington Capitals"/>
+    <s v="Capital One Arena"/>
+    <s v="Washington"/>
+    <x v="3"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <s v="Washington Wizards"/>
+    <s v="Capital One Arena"/>
+    <s v="Washington"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Washington Nationals"/>
+    <s v="Nationals Park"/>
+    <s v="Washington"/>
+    <x v="3"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Florida Panthers"/>
+    <s v="FLA Live Arena"/>
+    <s v="Sunrise"/>
+    <x v="4"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <s v="Jacksonville Jaguars"/>
+    <s v="TIAA Bank Field"/>
+    <s v="Jacksonville"/>
+    <x v="4"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="Miami Dolphins"/>
+    <s v="Hard Rock Stadium"/>
+    <s v="Miami Gardens"/>
+    <x v="4"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="Miami Heat"/>
+    <s v="Kaseya Center"/>
+    <s v="Miami"/>
+    <x v="4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Inter Miami CF"/>
+    <s v="DRV PNK Stadium"/>
+    <s v="Fort Lauderdale"/>
+    <x v="4"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="Miami Marlins"/>
+    <s v="loanDepot Park"/>
+    <s v="Miami"/>
+    <x v="4"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Orlando City SC"/>
+    <s v="Exploria Stadium"/>
+    <s v="Orlando"/>
+    <x v="4"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="Orlando Magic"/>
+    <s v="Amway Center"/>
+    <s v="Orlando"/>
+    <x v="4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Tampa Bay Buccaneers"/>
+    <s v="Raymond James Stadium"/>
+    <s v="Tampa"/>
+    <x v="4"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="Tampa Bay Lightning"/>
+    <s v="Amalie Arena"/>
+    <s v="Tampa"/>
+    <x v="4"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <s v="Tampa Bay Rays"/>
+    <s v="Tropicana Field"/>
+    <s v="St. Petersburg"/>
+    <x v="4"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Atlanta Falcons"/>
+    <s v="Mercedes-Benz Stadium"/>
+    <s v="Atlanta"/>
+    <x v="5"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="Atlanta United FC"/>
+    <s v="Mercedes-Benz Stadium"/>
+    <s v="Atlanta"/>
+    <x v="5"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="Atlanta Braves"/>
+    <s v="Truist Park"/>
+    <s v="Cumberland"/>
+    <x v="5"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Atlanta Hawks"/>
+    <s v="State Farm Arena"/>
+    <s v="Atlanta"/>
+    <x v="5"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Chicago Blackhawks"/>
+    <s v="United Center"/>
+    <s v="Chicago"/>
+    <x v="6"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <s v="Chicago Bulls"/>
+    <s v="United Center"/>
+    <s v="Chicago"/>
+    <x v="6"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Chicago Cubs"/>
+    <s v="Wrigley Field"/>
+    <s v="Chicago"/>
+    <x v="6"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Chicago Fire FC"/>
+    <s v="Soldier Field"/>
+    <s v="Chicago"/>
+    <x v="6"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="Chicago White Sox"/>
+    <s v="Guaranteed Rate Field"/>
+    <s v="Chicago"/>
+    <x v="6"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Chicago Bears"/>
+    <s v="Soldier Field"/>
+    <s v="Chicago"/>
+    <x v="6"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="Indiana Pacers"/>
+    <s v="Gainbridge Fieldhouse"/>
+    <s v="Indianapolis"/>
+    <x v="7"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Indianapolis Colts"/>
+    <s v="Lucas Oil Stadium"/>
+    <s v="Indianapolis"/>
+    <x v="7"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="Sporting Kansas City"/>
+    <s v="Children's Mercy Park"/>
+    <s v="Kansas City"/>
+    <x v="8"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="New Orleans Saints"/>
+    <s v="Caesars Superdome"/>
+    <s v="New Orleans"/>
+    <x v="9"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="New Orleans Pelicans"/>
+    <s v="Smoothie King Center"/>
+    <s v="New Orleans"/>
+    <x v="9"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Washington Commanders"/>
+    <s v="FedExField"/>
+    <s v="Landover"/>
+    <x v="10"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="Baltimore Orioles"/>
+    <s v="Oriole Park at Camden Yards"/>
+    <s v="Baltimore"/>
+    <x v="10"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Baltimore Ravens"/>
+    <s v="M&amp;T Bank Stadium"/>
+    <s v="Baltimore"/>
+    <x v="10"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="Boston Bruins"/>
+    <s v="TD Garden"/>
+    <s v="Boston"/>
+    <x v="11"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <s v="Boston Celtics"/>
+    <s v="TD Garden"/>
+    <s v="Boston"/>
+    <x v="11"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Boston Red Sox"/>
+    <s v="Fenway Park"/>
+    <s v="Boston"/>
+    <x v="11"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="New England Patriots"/>
+    <s v="Gillette Stadium"/>
+    <s v="Foxborough"/>
+    <x v="11"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="New England Revolution"/>
+    <s v="Gillette Stadium"/>
+    <s v="Foxborough"/>
+    <x v="11"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="Detroit Red Wings"/>
+    <s v="Little Caesars Arena"/>
+    <s v="Detroit"/>
+    <x v="12"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <s v="Detroit Tigers"/>
+    <s v="Comerica Park"/>
+    <s v="Detroit"/>
+    <x v="12"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Detroit Pistons"/>
+    <s v="Little Caesars Arena"/>
+    <s v="Detroit"/>
+    <x v="12"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Detroit Lions"/>
+    <s v="Ford Field"/>
+    <s v="Detroit"/>
+    <x v="12"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="Minnesota Timberwolves"/>
+    <s v="Target Center"/>
+    <s v="Minneapolis"/>
+    <x v="13"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Minnesota United FC"/>
+    <s v="Allianz Field"/>
+    <s v="St. Paul"/>
+    <x v="13"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="Minnesota Vikings"/>
+    <s v="U.S. Bank Stadium"/>
+    <s v="Minneapolis"/>
+    <x v="13"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="Minnesota Wild"/>
+    <s v="Xcel Energy Center"/>
+    <s v="St. Paul"/>
+    <x v="13"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <s v="Minnesota Twins"/>
+    <s v="Target Field"/>
+    <s v="Minneapolis"/>
+    <x v="13"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Kansas City Royals"/>
+    <s v="Kauffman Stadium"/>
+    <s v="Kansas City"/>
+    <x v="14"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="St. Louis Blues"/>
+    <s v="Enterprise Center"/>
+    <s v="St. Louis"/>
+    <x v="14"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <s v="St. Louis Cardinals"/>
+    <s v="Busch Stadium"/>
+    <s v="St. Louis"/>
+    <x v="14"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="St. Louis City SC"/>
+    <s v="CityPark"/>
+    <s v="St. Louis"/>
+    <x v="14"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="Kansas City Chiefs"/>
+    <s v="Arrowhead Stadium"/>
+    <s v="Kansas City"/>
+    <x v="14"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="Vegas Golden Knights"/>
+    <s v="T-Mobile Arena"/>
+    <s v="Paradise"/>
+    <x v="15"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <s v="Las Vegas Raiders"/>
+    <s v="Allegiant Stadium"/>
+    <s v="Paradise"/>
+    <x v="15"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="New York Giants"/>
+    <s v="MetLife Stadium"/>
+    <s v="East Rutherford"/>
+    <x v="16"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="New York Jets"/>
+    <s v="MetLife Stadium"/>
+    <s v="East Rutherford"/>
+    <x v="16"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="New York Red Bulls"/>
+    <s v="Red Bull Arena"/>
+    <s v="Harrison"/>
+    <x v="16"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="New Jersey Devils"/>
+    <s v="Prudential Center"/>
+    <s v="Newark"/>
+    <x v="16"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <s v="Buffalo Bills"/>
+    <s v="Highmark Stadium"/>
+    <s v="Orchard Park"/>
+    <x v="17"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="Buffalo Sabres"/>
+    <s v="KeyBank Center"/>
+    <s v="Buffalo"/>
+    <x v="17"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <s v="New York City FC"/>
+    <s v="Yankee Stadium"/>
+    <s v="New York City"/>
+    <x v="17"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="New York Islanders"/>
+    <s v="UBS Arena"/>
+    <s v="Elmont"/>
+    <x v="17"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <s v="New York Knicks"/>
+    <s v="Madison Square Garden"/>
+    <s v="New York City"/>
+    <x v="17"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="New York Mets"/>
+    <s v="Citi Field"/>
+    <s v="New York City"/>
+    <x v="17"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="New York Rangers"/>
+    <s v="Madison Square Garden"/>
+    <s v="New York City"/>
+    <x v="17"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <s v="New York Yankees"/>
+    <s v="Yankee Stadium"/>
+    <s v="New York City"/>
+    <x v="17"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Brooklyn Nets"/>
+    <s v="Barclays Center"/>
+    <s v="New York City"/>
+    <x v="17"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Carolina Panthers"/>
+    <s v="Bank of America Stadium"/>
+    <s v="Charlotte"/>
+    <x v="18"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="Charlotte Hornets"/>
+    <s v="Spectrum Center"/>
+    <s v="Charlotte"/>
+    <x v="18"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Charlotte FC"/>
+    <s v="Bank of America Stadium"/>
+    <s v="Charlotte"/>
+    <x v="18"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="Carolina Hurricanes"/>
+    <s v="PNC Arena"/>
+    <s v="Raleigh"/>
+    <x v="18"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <s v="Cincinnati Bengals"/>
+    <s v="Paycor Stadium"/>
+    <s v="Cincinnati"/>
+    <x v="19"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="Cincinnati Reds"/>
+    <s v="Great American Ball Park"/>
+    <s v="Cincinnati"/>
+    <x v="19"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="FC Cincinnati"/>
+    <s v="TQL Stadium"/>
+    <s v="Cincinnati"/>
+    <x v="19"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="Cleveland Cavaliers"/>
+    <s v="Rocket Mortgage FieldHouse"/>
+    <s v="Cleveland"/>
+    <x v="19"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Columbus Blue Jackets"/>
+    <s v="Nationwide Arena"/>
+    <s v="Columbus"/>
+    <x v="19"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <s v="Columbus Crew SC"/>
+    <s v="Lower.com Field"/>
+    <s v="Columbus"/>
+    <x v="19"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="Cleveland Browns"/>
+    <s v="FirstEnergy Stadium"/>
+    <s v="Cleveland"/>
+    <x v="19"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="Cleveland Guardians"/>
+    <s v="Progressive Field"/>
+    <s v="Cleveland"/>
+    <x v="19"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Oklahoma City Thunder"/>
+    <s v="Paycom Center"/>
+    <s v="Oklahoma City"/>
+    <x v="20"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Portland Trail Blazers"/>
+    <s v="Moda Center"/>
+    <s v="Portland"/>
+    <x v="21"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Portland Timbers"/>
+    <s v="Providence Park"/>
+    <s v="Portland"/>
+    <x v="21"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="Philadelphia Eagles"/>
+    <s v="Lincoln Financial Field"/>
+    <s v="Philadelphia"/>
+    <x v="22"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="Philadelphia Flyers"/>
+    <s v="Wells Fargo Center"/>
+    <s v="Philadelphia"/>
+    <x v="22"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <s v="Philadelphia Phillies"/>
+    <s v="Citizens Bank Park"/>
+    <s v="Philadelphia"/>
+    <x v="22"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Philadelphia Union"/>
+    <s v="Subaru Park"/>
+    <s v="Chester"/>
+    <x v="22"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="Pittsburgh Penguins"/>
+    <s v="PPG Paints Arena"/>
+    <s v="Pittsburgh"/>
+    <x v="22"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <s v="Pittsburgh Pirates"/>
+    <s v="PNC Park"/>
+    <s v="Pittsburgh"/>
+    <x v="22"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Pittsburgh Steelers"/>
+    <s v="Acrisure Stadium"/>
+    <s v="Pittsburgh"/>
+    <x v="22"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="Philadelphia 76ers"/>
+    <s v="Wells Fargo Center"/>
+    <s v="Philadelphia"/>
+    <x v="22"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Nashville Predators"/>
+    <s v="Bridgestone Arena"/>
+    <s v="Nashville"/>
+    <x v="23"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <s v="Nashville SC"/>
+    <s v="Geodis Park"/>
+    <s v="Nashville"/>
+    <x v="23"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="Tennessee Titans"/>
+    <s v="Nissan Stadium"/>
+    <s v="Nashville"/>
+    <x v="23"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="Memphis Grizzlies"/>
+    <s v="FedExForum"/>
+    <s v="Memphis"/>
+    <x v="23"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="FC Dallas"/>
+    <s v="Toyota Stadium"/>
+    <s v="Frisco"/>
+    <x v="24"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="Dallas Cowboys"/>
+    <s v="AT&amp;T Stadium"/>
+    <s v="Arlington"/>
+    <x v="24"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="Dallas Mavericks"/>
+    <s v="American Airlines Center"/>
+    <s v="Dallas"/>
+    <x v="24"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Houston Texans"/>
+    <s v="NRG Stadium"/>
+    <s v="Houston"/>
+    <x v="24"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="Houston Astros"/>
+    <s v="Minute Maid Park"/>
+    <s v="Houston"/>
+    <x v="24"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Austin FC"/>
+    <s v="Q2 Stadium"/>
+    <s v="Austin"/>
+    <x v="24"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="Houston Dynamo FC"/>
+    <s v="Shell Energy Stadium"/>
+    <s v="Houston"/>
+    <x v="24"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="San Antonio Spurs"/>
+    <s v="AT&amp;T Center"/>
+    <s v="San Antonio"/>
+    <x v="24"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Dallas Stars"/>
+    <s v="American Airlines Center"/>
+    <s v="Dallas"/>
+    <x v="24"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <s v="Houston Rockets"/>
+    <s v="Toyota Center"/>
+    <s v="Houston"/>
+    <x v="24"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Texas Rangers"/>
+    <s v="Globe Life Field"/>
+    <s v="Arlington"/>
+    <x v="24"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Real Salt Lake"/>
+    <s v="Rio Tinto Stadium"/>
+    <s v="Sandy"/>
+    <x v="25"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="Utah Jazz"/>
+    <s v="Vivint Arena"/>
+    <s v="Salt Lake City"/>
+    <x v="25"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Seattle Mariners"/>
+    <s v="T-Mobile Park"/>
+    <s v="Seattle"/>
+    <x v="26"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Seattle Seahawks"/>
+    <s v="Lumen Field"/>
+    <s v="Seattle"/>
+    <x v="26"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="Seattle Sounders FC"/>
+    <s v="Lumen Field"/>
+    <s v="Seattle"/>
+    <x v="26"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="Seattle Kraken"/>
+    <s v="Climate Pledge Arena"/>
+    <s v="Seattle"/>
+    <x v="26"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <s v="Green Bay Packers"/>
+    <s v="Lambeau Field"/>
+    <s v="Green Bay"/>
+    <x v="27"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="Milwaukee Bucks"/>
+    <s v="Fiserv Forum"/>
+    <s v="Milwaukee"/>
+    <x v="27"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Milwaukee Brewers"/>
+    <s v="American Family Field"/>
+    <s v="Milwaukee"/>
+    <x v="27"/>
+    <x v="0"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E59EB246-0424-4285-A453-915C4A864387}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:G33" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="5">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0" sortType="descending">
+      <items count="29">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="4" count="1" selected="0">
+              <x v="4"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="4"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="29">
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="24"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="23"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="26"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i>
+      <x v="25"/>
+    </i>
+    <i>
+      <x v="21"/>
+    </i>
+    <i>
+      <x v="27"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="4"/>
+  </colFields>
+  <colItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Team" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1509,11 +2783,657 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{270E73BC-0FB8-4DDB-8096-284CE798888B}">
+  <dimension ref="A3:G33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="17.61328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.4609375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.3828125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.53515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.23046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.69140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A3" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A4" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="3">
+        <v>5</v>
+      </c>
+      <c r="C5" s="3">
+        <v>4</v>
+      </c>
+      <c r="D5" s="3">
+        <v>4</v>
+      </c>
+      <c r="E5" s="3">
+        <v>3</v>
+      </c>
+      <c r="F5" s="3">
+        <v>3</v>
+      </c>
+      <c r="G5" s="3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A6" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B6" s="3">
+        <v>2</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3">
+        <v>2</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3">
+        <v>3</v>
+      </c>
+      <c r="G6" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A7" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="B7" s="3">
+        <v>2</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1</v>
+      </c>
+      <c r="E7" s="3">
+        <v>2</v>
+      </c>
+      <c r="F7" s="3">
+        <v>2</v>
+      </c>
+      <c r="G7" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A8" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B8" s="3">
+        <v>2</v>
+      </c>
+      <c r="C8" s="3">
+        <v>2</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2</v>
+      </c>
+      <c r="E8" s="3">
+        <v>3</v>
+      </c>
+      <c r="F8" s="3">
+        <v>2</v>
+      </c>
+      <c r="G8" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A9" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="B9" s="3">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3">
+        <v>1</v>
+      </c>
+      <c r="G9" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A10" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="3">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1</v>
+      </c>
+      <c r="F10" s="3">
+        <v>1</v>
+      </c>
+      <c r="G10" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A11" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="B11" s="3">
+        <v>2</v>
+      </c>
+      <c r="C11" s="3">
+        <v>3</v>
+      </c>
+      <c r="D11" s="3">
+        <v>3</v>
+      </c>
+      <c r="E11" s="3">
+        <v>2</v>
+      </c>
+      <c r="F11" s="3">
+        <v>1</v>
+      </c>
+      <c r="G11" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A12" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3">
+        <v>1</v>
+      </c>
+      <c r="F12" s="3">
+        <v>1</v>
+      </c>
+      <c r="G12" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A13" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3">
+        <v>1</v>
+      </c>
+      <c r="F13" s="3">
+        <v>1</v>
+      </c>
+      <c r="G13" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A14" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3">
+        <v>1</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3">
+        <v>2</v>
+      </c>
+      <c r="F14" s="3">
+        <v>1</v>
+      </c>
+      <c r="G14" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A15" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3">
+        <v>1</v>
+      </c>
+      <c r="D15" s="3">
+        <v>1</v>
+      </c>
+      <c r="E15" s="3">
+        <v>1</v>
+      </c>
+      <c r="F15" s="3">
+        <v>1</v>
+      </c>
+      <c r="G15" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A16" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B16" s="3">
+        <v>2</v>
+      </c>
+      <c r="C16" s="3">
+        <v>1</v>
+      </c>
+      <c r="D16" s="3">
+        <v>1</v>
+      </c>
+      <c r="E16" s="3">
+        <v>1</v>
+      </c>
+      <c r="F16" s="3">
+        <v>1</v>
+      </c>
+      <c r="G16" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A17" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B17" s="3">
+        <v>2</v>
+      </c>
+      <c r="C17" s="3">
+        <v>2</v>
+      </c>
+      <c r="D17" s="3">
+        <v>1</v>
+      </c>
+      <c r="E17" s="3">
+        <v>2</v>
+      </c>
+      <c r="F17" s="3">
+        <v>1</v>
+      </c>
+      <c r="G17" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A18" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B18" s="3">
+        <v>1</v>
+      </c>
+      <c r="C18" s="3">
+        <v>1</v>
+      </c>
+      <c r="D18" s="3">
+        <v>1</v>
+      </c>
+      <c r="E18" s="3">
+        <v>1</v>
+      </c>
+      <c r="F18" s="3">
+        <v>1</v>
+      </c>
+      <c r="G18" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A19" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3">
+        <v>1</v>
+      </c>
+      <c r="D19" s="3">
+        <v>1</v>
+      </c>
+      <c r="E19" s="3">
+        <v>1</v>
+      </c>
+      <c r="F19" s="3">
+        <v>1</v>
+      </c>
+      <c r="G19" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A20" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B20" s="3">
+        <v>1</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3">
+        <v>1</v>
+      </c>
+      <c r="E20" s="3">
+        <v>1</v>
+      </c>
+      <c r="F20" s="3">
+        <v>1</v>
+      </c>
+      <c r="G20" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A21" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" s="3">
+        <v>1</v>
+      </c>
+      <c r="C21" s="3">
+        <v>1</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3">
+        <v>1</v>
+      </c>
+      <c r="F21" s="3">
+        <v>1</v>
+      </c>
+      <c r="G21" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="3">
+        <v>1</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3">
+        <v>1</v>
+      </c>
+      <c r="E22" s="3">
+        <v>1</v>
+      </c>
+      <c r="F22" s="3">
+        <v>1</v>
+      </c>
+      <c r="G22" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A23" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B23" s="3">
+        <v>1</v>
+      </c>
+      <c r="C23" s="3">
+        <v>1</v>
+      </c>
+      <c r="D23" s="3">
+        <v>1</v>
+      </c>
+      <c r="E23" s="3">
+        <v>1</v>
+      </c>
+      <c r="F23" s="3">
+        <v>1</v>
+      </c>
+      <c r="G23" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A24" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3">
+        <v>1</v>
+      </c>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A25" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3">
+        <v>1</v>
+      </c>
+      <c r="E25" s="3">
+        <v>1</v>
+      </c>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A26" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3">
+        <v>1</v>
+      </c>
+      <c r="E26" s="3">
+        <v>1</v>
+      </c>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A27" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3">
+        <v>1</v>
+      </c>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A28" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3">
+        <v>1</v>
+      </c>
+      <c r="D28" s="3">
+        <v>1</v>
+      </c>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A29" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3">
+        <v>1</v>
+      </c>
+      <c r="D29" s="3">
+        <v>1</v>
+      </c>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A30" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="B30" s="3">
+        <v>1</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3">
+        <v>1</v>
+      </c>
+      <c r="E30" s="3">
+        <v>1</v>
+      </c>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A31" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B31" s="3">
+        <v>1</v>
+      </c>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3">
+        <v>2</v>
+      </c>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A32" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B32" s="3">
+        <v>1</v>
+      </c>
+      <c r="C32" s="3">
+        <v>1</v>
+      </c>
+      <c r="D32" s="3">
+        <v>1</v>
+      </c>
+      <c r="E32" s="3">
+        <v>1</v>
+      </c>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A33" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="B33" s="3">
+        <v>29</v>
+      </c>
+      <c r="C33" s="3">
+        <v>27</v>
+      </c>
+      <c r="D33" s="3">
+        <v>29</v>
+      </c>
+      <c r="E33" s="3">
+        <v>32</v>
+      </c>
+      <c r="F33" s="3">
+        <v>25</v>
+      </c>
+      <c r="G33" s="3">
+        <v>142</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A079FD68-9614-40E7-A6E1-AACCA79FCE9E}">
   <dimension ref="A1:E143"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>